<commit_message>
pipesar2s left! 12/3/2024 4:44:00 PM
</commit_message>
<xml_diff>
--- a/config/nssar1o1ccp/timing_table.xlsx
+++ b/config/nssar1o1ccp/timing_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Item</t>
   </si>
@@ -46,16 +46,19 @@
     <t>CB1</t>
   </si>
   <si>
+    <t>OUT RST RMAJ RMIN2 SAM1F</t>
+  </si>
+  <si>
+    <t>MSB CHS12</t>
+  </si>
+  <si>
+    <t>LSB</t>
+  </si>
+  <si>
+    <t>AMP0 F0N1</t>
+  </si>
+  <si>
     <t>OUT RST RMAJ RMIN2 SAM1</t>
-  </si>
-  <si>
-    <t>MSB CHS</t>
-  </si>
-  <si>
-    <t>LSB</t>
-  </si>
-  <si>
-    <t>AMP0 F0N1</t>
   </si>
 </sst>
 </file>
@@ -423,12 +426,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="2" width="5.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="29.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="34.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="2" width="9.719285714285713" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="2" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="29.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="2" width="35.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="2" width="9.862142857142858" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="2" width="7.433571428571429" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="2" width="11.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
@@ -479,7 +482,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>

</xml_diff>